<commit_message>
updated some pictures, more to do
</commit_message>
<xml_diff>
--- a/color-testing/relevance.xlsx
+++ b/color-testing/relevance.xlsx
@@ -137,7 +137,7 @@
             <c:noEndCap val="1"/>
             <c:val val="5.0"/>
             <c:spPr>
-              <a:ln w="25400"/>
+              <a:ln w="19050"/>
             </c:spPr>
           </c:errBars>
           <c:cat>
@@ -176,22 +176,29 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="473311608"/>
-        <c:axId val="473307176"/>
+        <c:axId val="566533944"/>
+        <c:axId val="566537192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="473311608"/>
+        <c:axId val="566533944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2400" b="0" i="0">
+              <a:defRPr sz="1000" b="0" i="0">
                 <a:latin typeface="Arial"/>
                 <a:cs typeface="Neutra Text-Book"/>
               </a:defRPr>
@@ -199,26 +206,33 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473307176"/>
+        <c:crossAx val="566537192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="473307176"/>
+        <c:axId val="566537192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2400">
+              <a:defRPr sz="800">
                 <a:latin typeface="Arial"/>
                 <a:cs typeface="Arial"/>
               </a:defRPr>
@@ -226,13 +240,18 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473311608"/>
+        <c:crossAx val="566533944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -251,10 +270,10 @@
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -598,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>